<commit_message>
Calendar Modile Completed Successfully
</commit_message>
<xml_diff>
--- a/Data/ConfigData/CalendarConfig.xlsx
+++ b/Data/ConfigData/CalendarConfig.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>TestId</t>
   </si>
@@ -82,7 +82,7 @@
     <t>calendar_001</t>
   </si>
   <si>
-    <t>Leave application for employee through admin</t>
+    <t>Calendar Update</t>
   </si>
   <si>
     <t>CalendarData</t>
@@ -92,9 +92,6 @@
   </si>
   <si>
     <t>ResCalendar</t>
-  </si>
-  <si>
-    <t>ResLeaveMuster</t>
   </si>
 </sst>
 </file>
@@ -131,6 +128,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -138,31 +142,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -176,6 +158,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -184,24 +181,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -215,8 +212,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -231,6 +237,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -239,29 +259,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -269,7 +266,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -284,25 +281,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -314,157 +461,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -475,6 +472,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -493,21 +514,21 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -528,24 +549,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -561,66 +564,60 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -629,97 +626,97 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1048,8 +1045,8 @@
   <sheetPr/>
   <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4"/>
@@ -1176,7 +1173,7 @@
         <v>3</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>24</v>
@@ -1191,7 +1188,7 @@
         <v>1</v>
       </c>
       <c r="T2" s="2">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="U2" s="2">
         <v>1</v>

</xml_diff>